<commit_message>
"With Manage Resumes Side Test Cases"
</commit_message>
<xml_diff>
--- a/src/main/java/com/rqanrs/qa/testdata/login.xlsx
+++ b/src/main/java/com/rqanrs/qa/testdata/login.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Username</t>
   </si>
@@ -23,13 +23,16 @@
     <t>Password</t>
   </si>
   <si>
-    <t>sagar</t>
+    <t>vaishnavi@rezoomex.com</t>
   </si>
   <si>
-    <t>sagar123</t>
+    <t>vaishnavi@0363</t>
   </si>
   <si>
-    <t>sagarakshe</t>
+    <t>ankit@rezoomex.com</t>
+  </si>
+  <si>
+    <t>ankit@4625</t>
   </si>
 </sst>
 </file>
@@ -39,7 +42,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -60,6 +63,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,9 +114,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -129,13 +143,13 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.2091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0969387755102"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -148,22 +162,26 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>1</v>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="vaishnavi@rezoomex.com"/>
+    <hyperlink ref="A3" r:id="rId2" display="ankit@rezoomex.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>